<commit_message>
update rev 5 controls to final release (no longer FPD)
</commit_message>
<xml_diff>
--- a/frameworks/nist800-53-r5/nist800-53-r5-mappings.xlsx
+++ b/frameworks/nist800-53-r5/nist800-53-r5-mappings.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -54,18 +54,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F153"/>
+  <dimension ref="A1:F151"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1045,12 +1045,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>AC-2(14)</t>
+          <t>AC-3</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Account Management | Prohibit Specific Account Types</t>
+          <t>Access Enforcement</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1077,12 +1077,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>AC-3</t>
+          <t>AC-3(1)</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Access Enforcement</t>
+          <t>Access Enforcement | Restricted Access to Privileged Functions</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1109,12 +1109,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>AC-3(1)</t>
+          <t>AC-3(2)</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Access Enforcement | Restricted Access to Privileged Functions</t>
+          <t>Access Enforcement | Dual Authorization</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1141,12 +1141,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>AC-3(2)</t>
+          <t>AC-3(3)</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Access Enforcement | Dual Authorization</t>
+          <t>Access Enforcement | Mandatory Access Control</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1173,12 +1173,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>AC-3(3)</t>
+          <t>AC-3(4)</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Access Enforcement | Mandatory Access Control</t>
+          <t>Access Enforcement | Discretionary Access Control</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1205,12 +1205,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>AC-3(4)</t>
+          <t>AC-3(5)</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Access Enforcement | Discretionary Access Control</t>
+          <t>Access Enforcement | Security-relevant Information</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1237,12 +1237,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>AC-3(5)</t>
+          <t>AC-3(6)</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Access Enforcement | Security-relevant Information</t>
+          <t>Access Enforcement | Protection of User and System Information</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1269,12 +1269,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>AC-3(6)</t>
+          <t>AC-3(7)</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Access Enforcement | Protection of User and System Information</t>
+          <t>Access Enforcement | Role-based Access Control</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1301,12 +1301,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>AC-3(7)</t>
+          <t>AC-3(8)</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Access Enforcement | Role-based Access Control</t>
+          <t>Access Enforcement | Revocation of Access Authorizations</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1333,12 +1333,12 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>AC-3(8)</t>
+          <t>AC-3(9)</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Access Enforcement | Revocation of Access Authorizations</t>
+          <t>Access Enforcement | Controlled Release</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1365,12 +1365,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>AC-3(9)</t>
+          <t>AC-3(10)</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Access Enforcement | Controlled Release</t>
+          <t>Access Enforcement | Audited Override of Access Control Mechanisms</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1397,12 +1397,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>AC-3(10)</t>
+          <t>AC-3(11)</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Access Enforcement | Audited Override of Access Control Mechanisms</t>
+          <t>Access Enforcement | Restrict Access to Specific Information Types</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1429,12 +1429,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>AC-3(11)</t>
+          <t>AC-3(12)</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Access Enforcement | Restrict Access to Specific Information Types</t>
+          <t>Access Enforcement | Assert and Enforce Application Access</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1461,12 +1461,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>AC-3(12)</t>
+          <t>AC-3(13)</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Access Enforcement | Assert and Enforce Application Access</t>
+          <t>Access Enforcement | Attribute-based Access Control</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1493,12 +1493,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>AC-3(13)</t>
+          <t>AC-3(14)</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Access Enforcement | Attribute-based Access Control</t>
+          <t>Access Enforcement | Individual Access</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1525,12 +1525,12 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>AC-3(14)</t>
+          <t>AC-3(15)</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Access Enforcement | Individual Access</t>
+          <t>Access Enforcement | Discretionary and Mandatory Access Control</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1557,12 +1557,12 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>AC-3(15)</t>
+          <t>AC-4</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Access Enforcement | Discretionary and Mandatory Access Control</t>
+          <t>Information Flow Enforcement</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1589,12 +1589,12 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>AC-4</t>
+          <t>AC-4(1)</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Information Flow Enforcement</t>
+          <t>Information Flow Enforcement | Object Security and Privacy Attributes</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1621,12 +1621,12 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>AC-4(1)</t>
+          <t>AC-4(2)</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Information Flow Enforcement | Object Security and Privacy Attributes</t>
+          <t>Information Flow Enforcement | Processing Domains</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1653,12 +1653,12 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>AC-4(2)</t>
+          <t>AC-4(3)</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Information Flow Enforcement | Processing Domains</t>
+          <t>Information Flow Enforcement | Dynamic Information Flow Control</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1685,12 +1685,12 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>AC-4(3)</t>
+          <t>AC-4(4)</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Information Flow Enforcement | Dynamic Information Flow Control</t>
+          <t>Information Flow Enforcement | Flow Control of Encrypted Information</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1717,12 +1717,12 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>AC-4(4)</t>
+          <t>AC-4(5)</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Information Flow Enforcement | Flow Control of Encrypted Information</t>
+          <t>Information Flow Enforcement | Embedded Data Types</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1749,12 +1749,12 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>AC-4(5)</t>
+          <t>AC-4(6)</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Information Flow Enforcement | Embedded Data Types</t>
+          <t>Information Flow Enforcement | Metadata</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1781,12 +1781,12 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>AC-4(6)</t>
+          <t>AC-4(7)</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Information Flow Enforcement | Metadata</t>
+          <t>Information Flow Enforcement | One-way Flow Mechanisms</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1813,12 +1813,12 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>AC-4(7)</t>
+          <t>AC-4(8)</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Information Flow Enforcement | One-way Flow Mechanisms</t>
+          <t>Information Flow Enforcement | Security and Privacy Policy Filters</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1845,12 +1845,12 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>AC-4(8)</t>
+          <t>AC-4(9)</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Information Flow Enforcement | Security and Privacy Policy Filters</t>
+          <t>Information Flow Enforcement | Human Reviews</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1877,12 +1877,12 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>AC-4(9)</t>
+          <t>AC-4(10)</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Information Flow Enforcement | Human Reviews</t>
+          <t>Information Flow Enforcement | Enable and Disable Security or Privacy Policy Filters</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1909,12 +1909,12 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>AC-4(10)</t>
+          <t>AC-4(11)</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Information Flow Enforcement | Enable and Disable Security or Privacy Policy Filters</t>
+          <t>Information Flow Enforcement | Configuration of Security or Privacy Policy Filters</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1941,12 +1941,12 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>AC-4(11)</t>
+          <t>AC-4(12)</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Information Flow Enforcement | Configuration of Security or Privacy Policy Filters</t>
+          <t>Information Flow Enforcement | Data Type Identifiers</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1973,12 +1973,12 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>AC-4(12)</t>
+          <t>AC-4(13)</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Information Flow Enforcement | Data Type Identifiers</t>
+          <t>Information Flow Enforcement | Decomposition into Policy-relevant Subcomponents</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -2005,12 +2005,12 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>AC-4(13)</t>
+          <t>AC-4(14)</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Information Flow Enforcement | Decomposition into Policy-relevant Subcomponents</t>
+          <t>Information Flow Enforcement | Security or Privacy Policy Filter Constraints</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -2037,12 +2037,12 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>AC-4(14)</t>
+          <t>AC-4(15)</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Information Flow Enforcement | Security or Privacy Policy Filter Constraints</t>
+          <t>Information Flow Enforcement | Detection of Unsanctioned Information</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -2069,12 +2069,12 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>AC-4(15)</t>
+          <t>AC-4(16)</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Information Flow Enforcement | Detection of Unsanctioned Information</t>
+          <t>Information Flow Enforcement | Information Transfers on Interconnected Systems</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -2101,12 +2101,12 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>AC-4(16)</t>
+          <t>AC-4(17)</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Information Flow Enforcement | Information Transfers on Interconnected Systems</t>
+          <t>Information Flow Enforcement | Domain Authentication</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -2133,12 +2133,12 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>AC-4(17)</t>
+          <t>AC-4(18)</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Information Flow Enforcement | Domain Authentication</t>
+          <t>Information Flow Enforcement | Security Attribute Binding</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2165,12 +2165,12 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>AC-4(18)</t>
+          <t>AC-4(19)</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Information Flow Enforcement | Security Attribute Binding</t>
+          <t>Information Flow Enforcement | Validation of Metadata</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -2197,12 +2197,12 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>AC-4(19)</t>
+          <t>AC-4(20)</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Information Flow Enforcement | Validation of Metadata</t>
+          <t>Information Flow Enforcement | Approved Solutions</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -2229,12 +2229,12 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>AC-4(20)</t>
+          <t>AC-4(21)</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Information Flow Enforcement | Approved Solutions</t>
+          <t>Information Flow Enforcement | Physical or Logical Separation of Information Flows</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -2261,12 +2261,12 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>AC-4(21)</t>
+          <t>AC-4(22)</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Information Flow Enforcement | Physical or Logical Separation of Information Flows</t>
+          <t>Information Flow Enforcement | Access Only</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2293,12 +2293,12 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>AC-4(22)</t>
+          <t>AC-4(23)</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Information Flow Enforcement | Access Only</t>
+          <t>Information Flow Enforcement | Modify Non-releasable Information</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -2325,12 +2325,12 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>AC-4(23)</t>
+          <t>AC-4(24)</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Information Flow Enforcement | Modify Non-releasable Information</t>
+          <t>Information Flow Enforcement | Internal Normalized Format</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -2357,12 +2357,12 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>AC-4(24)</t>
+          <t>AC-4(25)</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Information Flow Enforcement | Internal Normalized Format</t>
+          <t>Information Flow Enforcement | Data Sanitization</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -2389,12 +2389,12 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>AC-4(25)</t>
+          <t>AC-4(26)</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Information Flow Enforcement | Data Sanitization</t>
+          <t>Information Flow Enforcement | Audit Filtering Actions</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2421,12 +2421,12 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>AC-4(26)</t>
+          <t>AC-4(27)</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Information Flow Enforcement | Audit Filtering Actions</t>
+          <t>Information Flow Enforcement | Redundant/independent Filtering Mechanisms</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -2453,12 +2453,12 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>AC-4(27)</t>
+          <t>AC-4(28)</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Information Flow Enforcement | Redundant/independent Filtering Mechanisms</t>
+          <t>Information Flow Enforcement | Linear Filter Pipelines</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -2485,12 +2485,12 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>AC-4(28)</t>
+          <t>AC-4(29)</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Information Flow Enforcement | Linear Filter Pipelines</t>
+          <t>Information Flow Enforcement | Filter Orchestration Engines</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -2517,12 +2517,12 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>AC-4(29)</t>
+          <t>AC-4(30)</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Information Flow Enforcement | Filter Orchestration Engines</t>
+          <t>Information Flow Enforcement | Filter Mechanisms Using Multiple Processes</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -2549,12 +2549,12 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>AC-4(30)</t>
+          <t>AC-4(31)</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Information Flow Enforcement | Filter Mechanisms Using Multiple Processes</t>
+          <t>Information Flow Enforcement | Failed Content Transfer Prevention</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -2581,12 +2581,12 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>AC-4(31)</t>
+          <t>AC-4(32)</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Information Flow Enforcement | Failed Content Transfer Prevention</t>
+          <t>Information Flow Enforcement | Process Requirements for Information Transfer</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -2613,12 +2613,12 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>AC-4(32)</t>
+          <t>AC-5</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Information Flow Enforcement | Process Requirements for Information Transfer</t>
+          <t>Separation of Duties</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -2645,12 +2645,12 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>AC-5</t>
+          <t>AC-6</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Separation of Duties</t>
+          <t>Least Privilege</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -2677,12 +2677,12 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>AC-6</t>
+          <t>AC-6(1)</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Least Privilege</t>
+          <t>Least Privilege | Authorize Access to Security Functions</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -2709,12 +2709,12 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>AC-6(1)</t>
+          <t>AC-6(2)</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Least Privilege | Authorize Access to Security Functions</t>
+          <t>Least Privilege | Non-privileged Access for Nonsecurity Functions</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -2741,12 +2741,12 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>AC-6(2)</t>
+          <t>AC-6(3)</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Least Privilege | Non-privileged Access for Nonsecurity Functions</t>
+          <t>Least Privilege | Network Access to Privileged Commands</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -2773,12 +2773,12 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>AC-6(3)</t>
+          <t>AC-6(4)</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Least Privilege | Network Access to Privileged Commands</t>
+          <t>Least Privilege | Separate Processing Domains</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -2805,12 +2805,12 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>AC-6(4)</t>
+          <t>AC-6(5)</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Least Privilege | Separate Processing Domains</t>
+          <t>Least Privilege | Privileged Accounts</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -2837,12 +2837,12 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>AC-6(5)</t>
+          <t>AC-6(6)</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Least Privilege | Privileged Accounts</t>
+          <t>Least Privilege | Privileged Access by Non-organizational Users</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -2869,12 +2869,12 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>AC-6(6)</t>
+          <t>AC-6(7)</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Least Privilege | Privileged Access by Non-organizational Users</t>
+          <t>Least Privilege | Review of User Privileges</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -2901,12 +2901,12 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>AC-6(7)</t>
+          <t>AC-6(8)</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Least Privilege | Review of User Privileges</t>
+          <t>Least Privilege | Privilege Levels for Code Execution</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -2933,12 +2933,12 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>AC-6(8)</t>
+          <t>AC-6(9)</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Least Privilege | Privilege Levels for Code Execution</t>
+          <t>Least Privilege | Log Use of Privileged Functions</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -2965,12 +2965,12 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>AC-6(9)</t>
+          <t>AC-6(10)</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Least Privilege | Log Use of Privileged Functions</t>
+          <t>Least Privilege | Prohibit Non-privileged Users from Executing Privileged Functions</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -2997,12 +2997,12 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>AC-6(10)</t>
+          <t>AC-7</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Least Privilege | Prohibit Non-privileged Users from Executing Privileged Functions</t>
+          <t>Unsuccessful Logon Attempts</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -3029,12 +3029,12 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>AC-7</t>
+          <t>AC-7(1)</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Unsuccessful Logon Attempts</t>
+          <t>Unsuccessful Logon Attempts | Automatic Account Lock</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -3061,12 +3061,12 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>AC-7(1)</t>
+          <t>AC-7(2)</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Unsuccessful Logon Attempts | Automatic Account Lock</t>
+          <t>Unsuccessful Logon Attempts | Purge or Wipe Mobile Device</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -3093,12 +3093,12 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>AC-7(2)</t>
+          <t>AC-7(3)</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Unsuccessful Logon Attempts | Purge or Wipe Mobile Device</t>
+          <t>Unsuccessful Logon Attempts | Biometric Attempt Limiting</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -3125,12 +3125,12 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>AC-7(3)</t>
+          <t>AC-7(4)</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Unsuccessful Logon Attempts | Biometric Attempt Limiting</t>
+          <t>Unsuccessful Logon Attempts | Use of Alternate Authentication Factor</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -3157,12 +3157,12 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>AC-7(4)</t>
+          <t>AC-8</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Unsuccessful Logon Attempts | Use of Alternate Factor</t>
+          <t>System Use Notification</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -3189,12 +3189,12 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>AC-8</t>
+          <t>AC-9</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>System Use Notification</t>
+          <t>Previous Logon Notification</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -3221,12 +3221,12 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>AC-9</t>
+          <t>AC-9(1)</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Previous Logon Notification</t>
+          <t>Previous Logon Notification | Unsuccessful Logons</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -3253,12 +3253,12 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>AC-9(1)</t>
+          <t>AC-9(2)</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Previous Logon Notification | Unsuccessful Logons</t>
+          <t>Previous Logon Notification | Successful and Unsuccessful Logons</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -3285,12 +3285,12 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>AC-9(2)</t>
+          <t>AC-9(3)</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Previous Logon Notification | Successful and Unsuccessful Logons</t>
+          <t>Previous Logon Notification | Notification of Account Changes</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -3317,12 +3317,12 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>AC-9(3)</t>
+          <t>AC-9(4)</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Previous Logon Notification | Notification of Account Changes</t>
+          <t>Previous Logon Notification | Additional Logon Information</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -3349,12 +3349,12 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>AC-9(4)</t>
+          <t>AC-10</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Previous Logon Notification | Additional Logon Information</t>
+          <t>Concurrent Session Control</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -3381,12 +3381,12 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>AC-10</t>
+          <t>AC-11</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Concurrent Session Control</t>
+          <t>Device Lock</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -3413,12 +3413,12 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>AC-11</t>
+          <t>AC-11(1)</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Device Lock</t>
+          <t>Device Lock | Pattern-hiding Displays</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -3445,12 +3445,12 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>AC-11(1)</t>
+          <t>AC-12</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Device Lock | Pattern-hiding Displays</t>
+          <t>Session Termination</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -3477,12 +3477,12 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>AC-12</t>
+          <t>AC-12(1)</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Session Termination</t>
+          <t>Session Termination | User-initiated Logouts</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -3509,12 +3509,12 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>AC-12(1)</t>
+          <t>AC-12(2)</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Session Termination | User-initiated Logouts</t>
+          <t>Session Termination | Termination Message</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -3541,12 +3541,12 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>AC-12(2)</t>
+          <t>AC-12(3)</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Session Termination | Termination Message</t>
+          <t>Session Termination | Timeout Warning Message</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -3573,12 +3573,12 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>AC-12(3)</t>
+          <t>AC-13</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Session Termination | Timeout Warning Message</t>
+          <t>Supervision and Review ' Access Control</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -3605,12 +3605,12 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>AC-13</t>
+          <t>AC-14</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Supervision and Review - Access Control</t>
+          <t>Permitted Actions Without Identification or Authentication</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -3637,12 +3637,12 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>AC-14</t>
+          <t>AC-14(1)</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Permitted Actions Without Identification or Authentication</t>
+          <t>Permitted Actions Without Identification or Authentication | Necessary Uses</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -3669,12 +3669,12 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>AC-14(1)</t>
+          <t>AC-15</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Permitted Actions Without Identification or Authentication | Necessary Uses</t>
+          <t>Automated Marking</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -3701,12 +3701,12 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>AC-15</t>
+          <t>AC-16</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Automated Marking</t>
+          <t>Security and Privacy Attributes</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -3733,12 +3733,12 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>AC-16</t>
+          <t>AC-16(1)</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Security and Privacy Attributes</t>
+          <t>Security and Privacy Attributes | Dynamic Attribute Association</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -3765,12 +3765,12 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>AC-16(1)</t>
+          <t>AC-16(2)</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Security and Privacy Attributes | Dynamic Attribute Association</t>
+          <t>Security and Privacy Attributes | Attribute Value Changes by Authorized Individuals</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -3797,12 +3797,12 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>AC-16(2)</t>
+          <t>AC-16(3)</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Security and Privacy Attributes | Attribute Value Changes by Authorized Individuals</t>
+          <t>Security and Privacy Attributes | Maintenance of Attribute Associations by System</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -3829,12 +3829,12 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>AC-16(3)</t>
+          <t>AC-16(4)</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Security and Privacy Attributes | Maintenance of Attribute Associations by System</t>
+          <t>Security and Privacy Attributes | Association of Attributes by Authorized Individuals</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -3861,12 +3861,12 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>AC-16(4)</t>
+          <t>AC-16(5)</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Security and Privacy Attributes | Association of Attributes by Authorized Individuals</t>
+          <t>Security and Privacy Attributes | Attribute Displays on Objects to Be Output</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -3893,12 +3893,12 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>AC-16(5)</t>
+          <t>AC-16(6)</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Security and Privacy Attributes | Attribute Displays for Output Devices</t>
+          <t>Security and Privacy Attributes | Maintenance of Attribute Association</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -3925,12 +3925,12 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>AC-16(6)</t>
+          <t>AC-16(7)</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Security and Privacy Attributes | Maintenance of Attribute Association by Organization</t>
+          <t>Security and Privacy Attributes | Consistent Attribute Interpretation</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -3957,12 +3957,12 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>AC-16(7)</t>
+          <t>AC-16(8)</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Security and Privacy Attributes | Consistent Attribute Interpretation</t>
+          <t>Security and Privacy Attributes | Association Techniques and Technologies</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -3989,12 +3989,12 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>AC-16(8)</t>
+          <t>AC-16(9)</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Security and Privacy Attributes | Association Techniques and Technologies</t>
+          <t>Security and Privacy Attributes | Attribute Reassignment ' Regrading Mechanisms</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
@@ -4021,12 +4021,12 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>AC-16(9)</t>
+          <t>AC-16(10)</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Security and Privacy Attributes | Attribute Reassignment - Regrading Mechanisms</t>
+          <t>Security and Privacy Attributes | Attribute Configuration by Authorized Individuals</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -4053,12 +4053,12 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>AC-16(10)</t>
+          <t>AC-17</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Security and Privacy Attributes | Attribute Configuration by Authorized Individuals</t>
+          <t>Remote Access</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -4085,12 +4085,12 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>AC-17</t>
+          <t>AC-17(1)</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Remote Access</t>
+          <t>Remote Access | Monitoring and Control</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -4117,12 +4117,12 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>AC-17(1)</t>
+          <t>AC-17(2)</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Remote Access | Monitoring and Control</t>
+          <t>Remote Access | Protection of Confidentiality and Integrity Using Encryption</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
@@ -4149,12 +4149,12 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>AC-17(2)</t>
+          <t>AC-17(3)</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Remote Access | Protection of Confidentiality and Integrity Using Encryption</t>
+          <t>Remote Access | Managed Access Control Points</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
@@ -4181,12 +4181,12 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>AC-17(3)</t>
+          <t>AC-17(4)</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Remote Access | Managed Access Control Points</t>
+          <t>Remote Access | Privileged Commands and Access</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
@@ -4213,12 +4213,12 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>AC-17(4)</t>
+          <t>AC-17(5)</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Remote Access | Privileged Commands and Access</t>
+          <t>Remote Access | Monitoring for Unauthorized Connections</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
@@ -4245,12 +4245,12 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>AC-17(5)</t>
+          <t>AC-17(6)</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Remote Access | Monitoring for Unauthorized Connections</t>
+          <t>Remote Access | Protection of Mechanism Information</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
@@ -4277,12 +4277,12 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>AC-17(6)</t>
+          <t>AC-17(7)</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Remote Access | Protection of Mechanism Information</t>
+          <t>Remote Access | Additional Protection for Security Function Access</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
@@ -4309,12 +4309,12 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>AC-17(7)</t>
+          <t>AC-17(8)</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Remote Access | Additional Protection for Security Function Access</t>
+          <t>Remote Access | Disable Nonsecure Network Protocols</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
@@ -4341,12 +4341,12 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>AC-17(8)</t>
+          <t>AC-17(9)</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Remote Access | Disable Nonsecure Network Protocols</t>
+          <t>Remote Access | Disconnect or Disable Access</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
@@ -4373,12 +4373,12 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>AC-17(9)</t>
+          <t>AC-17(10)</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Remote Access | Disconnect or Disable Access</t>
+          <t>Remote Access | Authenticate Remote Commands</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -4405,12 +4405,12 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>AC-17(10)</t>
+          <t>AC-18</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>Remote Access | Authenticate Remote Commands</t>
+          <t>Wireless Access</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
@@ -4437,12 +4437,12 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>AC-18</t>
+          <t>AC-18(1)</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Wireless Access</t>
+          <t>Wireless Access | Authentication and Encryption</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
@@ -4469,12 +4469,12 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>AC-18(1)</t>
+          <t>AC-18(2)</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>Wireless Access | Authentication and Encryption</t>
+          <t>Wireless Access | Monitoring Unauthorized Connections</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
@@ -4501,12 +4501,12 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>AC-18(2)</t>
+          <t>AC-18(3)</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>Wireless Access | Monitoring Unauthorized Connections</t>
+          <t>Wireless Access | Disable Wireless Networking</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
@@ -4533,12 +4533,12 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>AC-18(3)</t>
+          <t>AC-18(4)</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Wireless Access | Disable Wireless Networking</t>
+          <t>Wireless Access | Restrict Configurations by Users</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
@@ -4565,12 +4565,12 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>AC-18(4)</t>
+          <t>AC-18(5)</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Wireless Access | Restrict Configurations by Users</t>
+          <t>Wireless Access | Antennas and Transmission Power Levels</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
@@ -4597,12 +4597,12 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>AC-18(5)</t>
+          <t>AC-19</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Wireless Access | Antennas and Transmission Power Levels</t>
+          <t>Access Control for Mobile Devices</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
@@ -4629,12 +4629,12 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>AC-19</t>
+          <t>AC-19(1)</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Access Control for Mobile Devices</t>
+          <t>Access Control for Mobile Devices | Use of Writable and Portable Storage Devices</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
@@ -4661,12 +4661,12 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>AC-19(1)</t>
+          <t>AC-19(2)</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>Access Control for Mobile Devices | Use of Writable and Portable Storage Devices</t>
+          <t>Access Control for Mobile Devices | Use of Personally Owned Portable Storage Devices</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
@@ -4693,12 +4693,12 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>AC-19(2)</t>
+          <t>AC-19(3)</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>Access Control for Mobile Devices | Use of Personally Owned Portable Storage Devices</t>
+          <t>Access Control for Mobile Devices | Use of Portable Storage Devices with No Identifiable Owner</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
@@ -4725,12 +4725,12 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>AC-19(3)</t>
+          <t>AC-19(4)</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>Access Control for Mobile Devices | Use of Portable Storage Devices with No Identifiable Owner</t>
+          <t>Access Control for Mobile Devices | Restrictions for Classified Information</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
@@ -4757,12 +4757,12 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>AC-19(4)</t>
+          <t>AC-19(5)</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Access Control for Mobile Devices | Restrictions for Classified Information</t>
+          <t>Access Control for Mobile Devices | Full Device or Container-based Encryption</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
@@ -4789,12 +4789,12 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>AC-19(5)</t>
+          <t>AC-20</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Access Control for Mobile Devices | Full Device and Container-based Encryption</t>
+          <t>Use of External Systems</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
@@ -4821,12 +4821,12 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>AC-20</t>
+          <t>AC-20(1)</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>Use of External Systems</t>
+          <t>Use of External Systems | Limits on Authorized Use</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
@@ -4853,12 +4853,12 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>AC-20(1)</t>
+          <t>AC-20(2)</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>Use of External Systems | Limits on Authorized Use</t>
+          <t>Use of External Systems | Portable Storage Devices ' Restricted Use</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
@@ -4885,12 +4885,12 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>AC-20(2)</t>
+          <t>AC-20(3)</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>Use of External Systems | Portable Storage Devices - Restricted Use</t>
+          <t>Use of External Systems | Non-organizationally Owned Systems  ' Restricted Use</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
@@ -4917,12 +4917,12 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>AC-20(3)</t>
+          <t>AC-20(4)</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>Use of External Systems | Non-organizationally Owned Systems  - Restricted Use</t>
+          <t>Use of External Systems | Network Accessible Storage Devices ' Prohibited Use</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
@@ -4949,12 +4949,12 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>AC-20(4)</t>
+          <t>AC-20(5)</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>Use of External Systems | Network Accessible Storage Devices</t>
+          <t>Use of External Systems | Portable Storage Devices ' Prohibited Use</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
@@ -4981,12 +4981,12 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>AC-20(5)</t>
+          <t>AC-21</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>Use of External Systems | Portable Storage Devices - Prohibited Use</t>
+          <t>Information Sharing</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
@@ -5013,12 +5013,12 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>AC-20(6)</t>
+          <t>AC-21(1)</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>Use of External Systems | Non-organizationally Owned Systems - Prohibited Use</t>
+          <t>Information Sharing | Automated Decision Support</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
@@ -5045,12 +5045,12 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>AC-21</t>
+          <t>AC-21(2)</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>Information Sharing</t>
+          <t>Information Sharing | Information Search and Retrieval</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
@@ -5077,12 +5077,12 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>AC-21(1)</t>
+          <t>AC-22</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>Information Sharing | Automated Decision Support</t>
+          <t>Publicly Accessible Content</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
@@ -5109,12 +5109,12 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>AC-21(2)</t>
+          <t>AC-23</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>Information Sharing | Information Search and Retrieval</t>
+          <t>Data Mining Protection</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
@@ -5141,12 +5141,12 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>AC-22</t>
+          <t>AC-24</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>Publicly Accessible Content</t>
+          <t>Access Control Decisions</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
@@ -5173,12 +5173,12 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>AC-23</t>
+          <t>AC-24(1)</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>Data Mining Protection</t>
+          <t>Access Control Decisions | Transmit Access Authorization Information</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
@@ -5205,12 +5205,12 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>AC-24</t>
+          <t>AC-24(2)</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>Access Control Decisions</t>
+          <t>Access Control Decisions | No User or Process Identity</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
@@ -5237,12 +5237,12 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>AC-24(1)</t>
+          <t>AC-25</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>Access Control Decisions | Transmit Access Authorization Information</t>
+          <t>Reference Monitor</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
@@ -5266,71 +5266,7 @@
         </is>
       </c>
     </row>
-    <row r="152">
-      <c r="A152" t="inlineStr">
-        <is>
-          <t>AC-24(2)</t>
-        </is>
-      </c>
-      <c r="B152" t="inlineStr">
-        <is>
-          <t>Access Control Decisions | No User or Process Identity</t>
-        </is>
-      </c>
-      <c r="C152" t="inlineStr">
-        <is>
-          <t>mitigates</t>
-        </is>
-      </c>
-      <c r="D152" t="inlineStr">
-        <is>
-          <t>T1011</t>
-        </is>
-      </c>
-      <c r="E152" t="inlineStr">
-        <is>
-          <t>Exfiltration Over Other Network Medium</t>
-        </is>
-      </c>
-      <c r="F152" t="inlineStr">
-        <is>
-          <t xml:space="preserve">this row maps T1011 to everything in the access control category. </t>
-        </is>
-      </c>
-    </row>
-    <row r="153">
-      <c r="A153" t="inlineStr">
-        <is>
-          <t>AC-25</t>
-        </is>
-      </c>
-      <c r="B153" t="inlineStr">
-        <is>
-          <t>Reference Monitor</t>
-        </is>
-      </c>
-      <c r="C153" t="inlineStr">
-        <is>
-          <t>mitigates</t>
-        </is>
-      </c>
-      <c r="D153" t="inlineStr">
-        <is>
-          <t>T1011</t>
-        </is>
-      </c>
-      <c r="E153" t="inlineStr">
-        <is>
-          <t>Exfiltration Over Other Network Medium</t>
-        </is>
-      </c>
-      <c r="F153" t="inlineStr">
-        <is>
-          <t xml:space="preserve">this row maps T1011 to everything in the access control category. </t>
-        </is>
-      </c>
-    </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>